<commit_message>
Added operator number field
</commit_message>
<xml_diff>
--- a/server/OUTPUT_MetalPlan.xlsx
+++ b/server/OUTPUT_MetalPlan.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BUN023</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="G2" s="1" t="n">
-        <v>45675.34820555556</v>
+        <v>45689.10876496809</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>45677.02042777778</v>
+        <v>45691.64243497642</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45667</v>
+        <v>45635</v>
       </c>
     </row>
     <row r="3">
@@ -516,7 +516,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BUN005</t>
+          <t>BUN054</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -536,13 +536,13 @@
         </is>
       </c>
       <c r="G3" s="1" t="n">
-        <v>45675.10965111111</v>
+        <v>45688.16749069445</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>45677.56742888889</v>
+        <v>45690.62526847222</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.09236111111</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>140000</v>
+        <v>630000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -573,13 +573,13 @@
         </is>
       </c>
       <c r="G4" s="1" t="n">
-        <v>45674.10678555555</v>
+        <v>45686.84194322222</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>45674.81125777778</v>
+        <v>45690.23749933334</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.09236111111</v>
       </c>
     </row>
     <row r="5">
@@ -590,7 +590,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BUN025</t>
+          <t>BUN014</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>280000</v>
+        <v>420000</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -610,13 +610,13 @@
         </is>
       </c>
       <c r="G5" s="1" t="n">
-        <v>45675.79152444444</v>
+        <v>45688.00480643979</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>45677.40930222222</v>
+        <v>45690.46258421757</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.09236111111</v>
       </c>
     </row>
     <row r="6">
@@ -627,7 +627,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BUN011</t>
+          <t>BUN023</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>420000</v>
+        <v>560000</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -647,13 +647,13 @@
         </is>
       </c>
       <c r="G6" s="1" t="n">
-        <v>45675.48381915306</v>
+        <v>45686.87598655555</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>45677.94159693083</v>
+        <v>45690.17376433333</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.09236111111</v>
       </c>
     </row>
     <row r="7">
@@ -664,19 +664,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BUN015</t>
+          <t>BUN001</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>B0007X02500S023CU</t>
+          <t>B0007X02570S023CU</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>280000</v>
+        <v>420000</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -684,13 +684,13 @@
         </is>
       </c>
       <c r="G7" s="1" t="n">
-        <v>45676.26340277777</v>
+        <v>45687.80589760306</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>45677.88118055555</v>
+        <v>45690.14931651694</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="8">
@@ -701,19 +701,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BUN013</t>
+          <t>BUN015</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>B0007X02500S023CU</t>
+          <t>B0007X02570S023CU</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>140000</v>
+        <v>420000</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -721,13 +721,13 @@
         </is>
       </c>
       <c r="G8" s="1" t="n">
-        <v>45674.11265</v>
+        <v>45688.58053703333</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>45674.89042777778</v>
+        <v>45690.92395594722</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="9">
@@ -738,19 +738,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BUN023</t>
+          <t>BUN012</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>B0007X02500S023CU</t>
+          <t>B0007X02570S023CU</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>210000</v>
+        <v>560000</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -758,13 +758,13 @@
         </is>
       </c>
       <c r="G9" s="1" t="n">
-        <v>45674.08153888889</v>
+        <v>45687.09571595</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>45675.31042777777</v>
+        <v>45690.24005018889</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="10">
@@ -775,19 +775,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BUN006</t>
+          <t>BUN014</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>B0007X02500S023CU</t>
+          <t>B0007X02570S023CU</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>140000</v>
+        <v>171500</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -795,13 +795,13 @@
         </is>
       </c>
       <c r="G10" s="1" t="n">
-        <v>45674.13407777778</v>
+        <v>45686.9748115332</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>45674.91185555555</v>
+        <v>45687.94258421757</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="11">
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="G11" s="1" t="n">
-        <v>45674.94975483889</v>
+        <v>45686.99936222778</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>45678.09408907778</v>
+        <v>45690.14369646666</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="12">
@@ -849,7 +849,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BUN004</t>
+          <t>BUN003</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>560000</v>
+        <v>280000</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -869,13 +869,13 @@
         </is>
       </c>
       <c r="G12" s="1" t="n">
-        <v>45674.21689372777</v>
+        <v>45688.89269095</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>45677.36122796666</v>
+        <v>45690.43519453889</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="13">
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>591500</v>
+        <v>560000</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -906,13 +906,13 @@
         </is>
       </c>
       <c r="G13" s="1" t="n">
-        <v>45674.17091525542</v>
+        <v>45686.99936222778</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>45677.54143391479</v>
+        <v>45690.14369646666</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="14">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>420000</v>
+        <v>560000</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -943,13 +943,13 @@
         </is>
       </c>
       <c r="G14" s="1" t="n">
-        <v>45674.97118261667</v>
+        <v>45687.71223306111</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>45677.31460153055</v>
+        <v>45690.8565673</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="15">
@@ -960,7 +960,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BUN012</t>
+          <t>BUN004</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>420000</v>
+        <v>560000</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -980,13 +980,13 @@
         </is>
       </c>
       <c r="G15" s="1" t="n">
-        <v>45675.59020206111</v>
+        <v>45686.99936222778</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>45677.933620975</v>
+        <v>45690.14369646666</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="16">
@@ -997,19 +997,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BUN014</t>
+          <t>BUN015</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>B0007X02570S023CU</t>
+          <t>B0007X02500S023SN</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>560000</v>
+        <v>250000</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1017,13 +1017,13 @@
         </is>
       </c>
       <c r="G16" s="1" t="n">
-        <v>45674.21689372777</v>
+        <v>45687.07676552778</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>45677.36122796666</v>
+        <v>45688.52120997222</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.56458333333</v>
       </c>
     </row>
     <row r="17">
@@ -1034,19 +1034,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BUN003</t>
+          <t>BUN006</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>B0007X02570S023CU</t>
+          <t>B0007X02500S023SN</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>560000</v>
+        <v>131000</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1054,13 +1054,13 @@
         </is>
       </c>
       <c r="G17" s="1" t="n">
-        <v>45674.89144983889</v>
+        <v>45686.69551388889</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>45678.03578407778</v>
+        <v>45687.652906</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.56458333333</v>
       </c>
     </row>
     <row r="18">
@@ -1071,19 +1071,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BUN024</t>
+          <t>BUN005</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>B0007X02570S023CU</t>
+          <t>B0019X01560S023CU</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>420000</v>
+        <v>125000</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1091,13 +1091,13 @@
         </is>
       </c>
       <c r="G18" s="1" t="n">
-        <v>45674.87274111111</v>
+        <v>45689.22792711111</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>45677.30133277778</v>
+        <v>45689.92237155556</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45636.45486111111</v>
       </c>
     </row>
     <row r="19">
@@ -1112,15 +1112,15 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>B0007X02500S023SN</t>
+          <t>B0019X01560S023CU</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>250000</v>
+        <v>55000</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1128,13 +1128,13 @@
         </is>
       </c>
       <c r="G19" s="1" t="n">
-        <v>45674.08643055556</v>
+        <v>45686.73083333333</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>45675.530875</v>
+        <v>45687.03638888889</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45667.43958333333</v>
+        <v>45636.45486111111</v>
       </c>
     </row>
     <row r="20">
@@ -1145,19 +1145,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BUN015</t>
+          <t>BUN009</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>B0007X02500S023SN</t>
+          <t>B0019X01835S025CU</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>125000</v>
+        <v>570000</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1165,13 +1165,13 @@
         </is>
       </c>
       <c r="G20" s="1" t="n">
-        <v>45674.08173611111</v>
+        <v>45687.44077325361</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>45674.77618055556</v>
+        <v>45690.51148020917</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45667.43958333333</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="21">
@@ -1182,19 +1182,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BUN003</t>
+          <t>BUN010</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>B0007X02500S023SN</t>
+          <t>B0019X01835S025CU</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>6000</v>
+        <v>665000</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1202,13 +1202,13 @@
         </is>
       </c>
       <c r="G21" s="1" t="n">
-        <v>45674.02884722222</v>
+        <v>45687.00349772583</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>45674.06218055556</v>
+        <v>45690.59238648014</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45667.43958333333</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="22">
@@ -1219,19 +1219,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BUN037</t>
+          <t>BUN001</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>B0019X01560S023CU</t>
+          <t>B0019X01835S025CU</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>180000</v>
+        <v>190000</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1239,13 +1239,13 @@
         </is>
       </c>
       <c r="G22" s="1" t="n">
-        <v>45675.50750555556</v>
+        <v>45686.74859078139</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>45676.56306111111</v>
+        <v>45687.74657054195</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45667.45486111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="23">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BUN015</t>
+          <t>BUN002</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1268,7 +1268,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>190000</v>
+        <v>380000</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1276,13 +1276,13 @@
         </is>
       </c>
       <c r="G23" s="1" t="n">
-        <v>45674.82895833333</v>
+        <v>45688.4095328925</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>45676.20118055555</v>
+        <v>45690.44387625055</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="24">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BUN010</t>
+          <t>BUN011</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1313,13 +1313,13 @@
         </is>
       </c>
       <c r="G24" s="1" t="n">
-        <v>45674.61936717028</v>
+        <v>45687.30332828139</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>45678.20825592458</v>
+        <v>45690.8922170357</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="25">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BUN009</t>
+          <t>BUN025</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>665000</v>
+        <v>285000</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1350,13 +1350,13 @@
         </is>
       </c>
       <c r="G25" s="1" t="n">
-        <v>45674.5470056425</v>
+        <v>45688.12809330555</v>
       </c>
       <c r="H25" s="1" t="n">
-        <v>45678.13589439681</v>
+        <v>45690.62975997222</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="26">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BUN002</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>570000</v>
+        <v>285000</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1387,13 +1387,13 @@
         </is>
       </c>
       <c r="G26" s="1" t="n">
-        <v>45675.03906105916</v>
+        <v>45687.75282275</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>45678.10976801472</v>
+        <v>45690.25448941666</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="27">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BUN011</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1424,13 +1424,13 @@
         </is>
       </c>
       <c r="G27" s="1" t="n">
-        <v>45674.42361717028</v>
+        <v>45688.23861</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>45675.42159693084</v>
+        <v>45690.43416555555</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="28">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BUN001</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1453,7 +1453,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>631600</v>
+        <v>346600</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1461,13 +1461,13 @@
         </is>
       </c>
       <c r="G28" s="1" t="n">
-        <v>45674.35712361017</v>
+        <v>45687.18586941573</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>45677.77732550212</v>
+        <v>45689.05152591143</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="29">
@@ -1478,19 +1478,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BUN008</t>
+          <t>BUN011</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>B0019X01835S025CU</t>
+          <t>B0019X02230S027CU</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>665000</v>
+        <v>715000</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1498,13 +1498,13 @@
         </is>
       </c>
       <c r="G29" s="1" t="n">
-        <v>45674.66386550361</v>
+        <v>45686.73230555555</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>45678.25275425792</v>
+        <v>45687.26494444445</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="30">
@@ -1527,7 +1527,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>716000</v>
+        <v>325000</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1535,13 +1535,13 @@
         </is>
       </c>
       <c r="G30" s="1" t="n">
-        <v>45674.04759444445</v>
+        <v>45686.724975</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>45674.58098333333</v>
+        <v>45686.96511388889</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45667.54861111111</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="31">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BUN011</t>
+          <t>BUN003</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1564,7 +1564,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>455000</v>
+        <v>196000</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1572,13 +1572,13 @@
         </is>
       </c>
       <c r="G31" s="1" t="n">
-        <v>45674.04759444445</v>
+        <v>45686.76469722222</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>45674.38523333333</v>
+        <v>45688.48536388889</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>45667.54861111111</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="32">
@@ -1589,19 +1589,19 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BUN025</t>
+          <t>BUN005</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>B0019X02230S027CU</t>
+          <t>B0019X02570S030CU</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>65000</v>
+        <v>237500</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1609,13 +1609,13 @@
         </is>
       </c>
       <c r="G32" s="1" t="n">
-        <v>45674.28763555556</v>
+        <v>45687.76959377778</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>45674.82930222222</v>
+        <v>45689.17237155556</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>45667.54861111111</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="33">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BUN037</t>
+          <t>BUN002</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1638,7 +1638,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1646,13 +1646,13 @@
         </is>
       </c>
       <c r="G33" s="1" t="n">
-        <v>45674.61639444444</v>
+        <v>45687.19337127778</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>45675.48306111111</v>
+        <v>45688.37114905556</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>45668.57291666666</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="34">
@@ -1663,19 +1663,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BUN025</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>B0019X02570S030CU</t>
+          <t>B0019X03090S035CU</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>100000</v>
+        <v>87000</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1683,13 +1683,13 @@
         </is>
       </c>
       <c r="G34" s="1" t="n">
-        <v>45674.86263555555</v>
+        <v>45686.92582275</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>45675.72930222222</v>
+        <v>45687.68948941667</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>45668.57291666666</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="35">
@@ -1700,19 +1700,19 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BUN054</t>
+          <t>BUN009</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>B0019X02570S030CU</t>
+          <t>B0019X03090S035CU</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>237500</v>
+        <v>116000</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1720,13 +1720,13 @@
         </is>
       </c>
       <c r="G35" s="1" t="n">
-        <v>45675.11931513889</v>
+        <v>45686.91567275</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>45677.22348180556</v>
+        <v>45687.40238941667</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>45668.57291666666</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="36">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BUN008</t>
+          <t>BUN054</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1749,7 +1749,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>116000</v>
+        <v>58000</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1757,13 +1757,13 @@
         </is>
       </c>
       <c r="G36" s="1" t="n">
-        <v>45674.138765</v>
+        <v>45687.60260180556</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>45674.62548166667</v>
+        <v>45688.10526847222</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="37">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>BUN002</t>
+          <t>BUN025</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1786,7 +1786,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>203000</v>
+        <v>192500</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1794,13 +1794,13 @@
         </is>
       </c>
       <c r="G37" s="1" t="n">
-        <v>45674.14203555555</v>
+        <v>45686.91798219444</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>45675.00067722222</v>
+        <v>45688.06475997222</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="38">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BUN037</t>
+          <t>BUN003</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>47500</v>
+        <v>29000</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1831,13 +1831,13 @@
         </is>
       </c>
       <c r="G38" s="1" t="n">
-        <v>45674.141915</v>
+        <v>45688.51114166667</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>45674.55708166667</v>
+        <v>45688.83336388889</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="39">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>BUN002</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>87000</v>
+        <v>58000</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1868,13 +1868,13 @@
         </is>
       </c>
       <c r="G39" s="1" t="n">
-        <v>45675.51825958333</v>
+        <v>45686.91894330556</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>45676.53648180555</v>
+        <v>45687.15770997222</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="40">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BUN009</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1905,13 +1905,13 @@
         </is>
       </c>
       <c r="G40" s="1" t="n">
-        <v>45674.26985513889</v>
+        <v>45686.92221386111</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>45674.50862180556</v>
+        <v>45687.16098052778</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="41">
@@ -1922,19 +1922,19 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BUN003</t>
+          <t>BUN015</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>B0019X03090S035CU</t>
+          <t>B0019X03560S044CU</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>58000</v>
+        <v>9000</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1942,13 +1942,13 @@
         </is>
       </c>
       <c r="G41" s="1" t="n">
-        <v>45674.16190055555</v>
+        <v>45686.94620997222</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>45674.83212277778</v>
+        <v>45687.02120997222</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45638.76597222222</v>
       </c>
     </row>
     <row r="42">
@@ -1959,19 +1959,19 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>BUN001</t>
+          <t>BUN005</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>B0019X03090S035CU</t>
+          <t>B0037X02840S050CU</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>29000</v>
+        <v>132000</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1979,13 +1979,13 @@
         </is>
       </c>
       <c r="G42" s="1" t="n">
-        <v>45674.14203555555</v>
+        <v>45686.80211577778</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>45674.25682722222</v>
+        <v>45687.74737155555</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45638.84375</v>
       </c>
     </row>
     <row r="43">
@@ -1996,19 +1996,19 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BUN025</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>B0019X03560S044CU</t>
+          <t>B0037X02840S050CU</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>9000</v>
+        <v>48000</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2016,13 +2016,13 @@
         </is>
       </c>
       <c r="G43" s="1" t="n">
-        <v>45674.16930222222</v>
+        <v>45686.80883222222</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>45674.24430222222</v>
+        <v>45687.23016555556</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>45669.76597222222</v>
+        <v>45638.84375</v>
       </c>
     </row>
     <row r="44">
@@ -2033,19 +2033,19 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BUN005</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>B0037X02840S050CU</t>
+          <t>B0044X02910S050CU</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2053,13 +2053,13 @@
         </is>
       </c>
       <c r="G44" s="1" t="n">
-        <v>45674.17807911111</v>
+        <v>45686.83262513889</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>45674.50742888889</v>
+        <v>45686.88470847222</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>45669.84375</v>
+        <v>45639.95069444444</v>
       </c>
     </row>
     <row r="45">
@@ -2070,19 +2070,19 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>BUN054</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>B0037X02840S050CU</t>
+          <t>B0056X02930S060CU</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>80000</v>
+        <v>100100</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2090,13 +2090,13 @@
         </is>
       </c>
       <c r="G45" s="1" t="n">
-        <v>45674.78314847222</v>
+        <v>45686.83751847222</v>
       </c>
       <c r="H45" s="1" t="n">
-        <v>45675.49248180556</v>
+        <v>45687.58326847222</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>45669.84375</v>
+        <v>45640</v>
       </c>
     </row>
     <row r="46">
@@ -2107,19 +2107,19 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BUN009</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>B0044X02910S050CU</t>
+          <t>B0056X02930S060CU</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>7500</v>
+        <v>63000</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2127,13 +2127,13 @@
         </is>
       </c>
       <c r="G46" s="1" t="n">
-        <v>45674.20858847223</v>
+        <v>45687.40616555556</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>45674.26067180555</v>
+        <v>45688.15416555556</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>45669.95069444444</v>
+        <v>45640</v>
       </c>
     </row>
     <row r="47">
@@ -2156,7 +2156,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>72000</v>
+        <v>54000</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2164,13 +2164,13 @@
         </is>
       </c>
       <c r="G47" s="1" t="n">
-        <v>45674.51242888889</v>
+        <v>45687.22738355555</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>45675.04742888889</v>
+        <v>45687.62738355555</v>
       </c>
       <c r="I47" s="1" t="n">
-        <v>45670</v>
+        <v>45640</v>
       </c>
     </row>
     <row r="48">
@@ -2181,19 +2181,19 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BUN054</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>B0056X02930S060CU</t>
+          <t>B0084X02930S065CU</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>117000</v>
+        <v>14000</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2201,13 +2201,13 @@
         </is>
       </c>
       <c r="G48" s="1" t="n">
-        <v>45674.21348180556</v>
+        <v>45687.23638777778</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>45675.08598180555</v>
+        <v>45687.39816555555</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>45670</v>
+        <v>45640.10763888889</v>
       </c>
     </row>
     <row r="49">
@@ -2218,19 +2218,19 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>BUN005</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>B0056X02930S060CU</t>
+          <t>B0084X02930S065CU</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>28100</v>
+        <v>13900</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2238,13 +2238,13 @@
         </is>
       </c>
       <c r="G49" s="1" t="n">
-        <v>45674.20945958333</v>
+        <v>45687.12196688889</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>45676.64448180555</v>
+        <v>45687.22238355556</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>45670</v>
+        <v>45640.10763888889</v>
       </c>
     </row>
     <row r="50">
@@ -2255,19 +2255,19 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>B0084X02930S065CU</t>
+          <t>D07X01570CUSN</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>27900</v>
+        <v>285000</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2275,13 +2275,13 @@
         </is>
       </c>
       <c r="G50" s="1" t="n">
-        <v>45674.44390402778</v>
+        <v>45686.67066666667</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>45674.77248180556</v>
+        <v>45686.69566666667</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>45670.10763888889</v>
+        <v>45635</v>
       </c>
     </row>
     <row r="51">
@@ -2296,15 +2296,15 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>D07X01570CUSN</t>
+          <t>D07X02500CU</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>285000</v>
+        <v>2030000</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2312,13 +2312,13 @@
         </is>
       </c>
       <c r="G51" s="1" t="n">
-        <v>45674.004</v>
+        <v>45686.79529211111</v>
       </c>
       <c r="H51" s="1" t="n">
-        <v>45674.029</v>
+        <v>45686.89947544444</v>
       </c>
       <c r="I51" s="1" t="n">
-        <v>45667</v>
+        <v>45635.09236111111</v>
       </c>
     </row>
     <row r="52">
@@ -2333,15 +2333,15 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>D07X02500CU</t>
+          <t>D07X02570CU</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2030000</v>
+        <v>4091500</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2349,13 +2349,13 @@
         </is>
       </c>
       <c r="G52" s="1" t="n">
-        <v>45674.03195555555</v>
+        <v>45686.92156294444</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>45674.13613888889</v>
+        <v>45687.13288516667</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>45667.09236111111</v>
+        <v>45635.34652777778</v>
       </c>
     </row>
     <row r="53">
@@ -2366,19 +2366,19 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW001</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>D07X02570CU</t>
+          <t>D07X02500SN</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>4091500</v>
+        <v>250000</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2386,13 +2386,13 @@
         </is>
       </c>
       <c r="G53" s="1" t="n">
-        <v>45674.13909444444</v>
+        <v>45686.67027777778</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>45674.57540833333</v>
+        <v>45686.69284722222</v>
       </c>
       <c r="I53" s="1" t="n">
-        <v>45667.34652777778</v>
+        <v>45635.56458333333</v>
       </c>
     </row>
     <row r="54">
@@ -2403,7 +2403,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>MDW001</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>381000</v>
+        <v>131000</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2423,13 +2423,13 @@
         </is>
       </c>
       <c r="G54" s="1" t="n">
-        <v>45674.00361111111</v>
+        <v>45686.90211433333</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>45674.05236111111</v>
+        <v>45686.91860738889</v>
       </c>
       <c r="I54" s="1" t="n">
-        <v>45667.43958333333</v>
+        <v>45635.56458333333</v>
       </c>
     </row>
     <row r="55">
@@ -2460,13 +2460,13 @@
         </is>
       </c>
       <c r="G55" s="1" t="n">
-        <v>45674.02979166667</v>
+        <v>45686.69645833333</v>
       </c>
       <c r="H55" s="1" t="n">
-        <v>45674.05236111111</v>
+        <v>45686.71902777778</v>
       </c>
       <c r="I55" s="1" t="n">
-        <v>45667.45486111111</v>
+        <v>45636.45486111111</v>
       </c>
     </row>
     <row r="56">
@@ -2497,13 +2497,13 @@
         </is>
       </c>
       <c r="G56" s="1" t="n">
-        <v>45674.00361111111</v>
+        <v>45686.67027777778</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>45674.02618055556</v>
+        <v>45686.69284722222</v>
       </c>
       <c r="I56" s="1" t="n">
-        <v>45667.45486111111</v>
+        <v>45636.45486111111</v>
       </c>
     </row>
     <row r="57">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>3576600</v>
+        <v>380000</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2534,13 +2534,13 @@
         </is>
       </c>
       <c r="G57" s="1" t="n">
-        <v>45674.32410694444</v>
+        <v>45686.66814444445</v>
       </c>
       <c r="H57" s="1" t="n">
-        <v>45674.511125</v>
+        <v>45686.67738055556</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="58">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW002</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2563,7 +2563,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>190000</v>
+        <v>3386600</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2571,13 +2571,13 @@
         </is>
       </c>
       <c r="G58" s="1" t="n">
-        <v>45674.30956666666</v>
+        <v>45686.72103333334</v>
       </c>
       <c r="H58" s="1" t="n">
-        <v>45674.32210138889</v>
+        <v>45686.98075277778</v>
       </c>
       <c r="I58" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="59">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>D12X01835CU</t>
+          <t>D07X01835CU</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>3386600</v>
+        <v>1710000</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2608,13 +2608,13 @@
         </is>
       </c>
       <c r="G59" s="1" t="n">
-        <v>45674.05436666666</v>
+        <v>45686.98275833333</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>45674.31408611111</v>
+        <v>45687.06799444444</v>
       </c>
       <c r="I59" s="1" t="n">
-        <v>45667.46736111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="60">
@@ -2625,19 +2625,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>MDW003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>D07X02230CU</t>
+          <t>D07X01835CU</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1236000</v>
+        <v>1486600</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2645,13 +2645,13 @@
         </is>
       </c>
       <c r="G60" s="1" t="n">
-        <v>45674.00101111111</v>
+        <v>45686.7122125</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>45674.03665277778</v>
+        <v>45686.79233655555</v>
       </c>
       <c r="I60" s="1" t="n">
-        <v>45667.54861111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="61">
@@ -2662,19 +2662,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>MDW003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>D12X02230CU</t>
+          <t>D12X01835CU</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1236000</v>
+        <v>190000</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2682,13 +2682,13 @@
         </is>
       </c>
       <c r="G61" s="1" t="n">
-        <v>45674.03766388889</v>
+        <v>45686.69767222222</v>
       </c>
       <c r="H61" s="1" t="n">
-        <v>45674.10995833333</v>
+        <v>45686.71020694444</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>45667.54861111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="62">
@@ -2699,19 +2699,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>D07X02570CU</t>
+          <t>D07X02230CU</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>437500</v>
+        <v>1236000</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2719,13 +2719,13 @@
         </is>
       </c>
       <c r="G62" s="1" t="n">
-        <v>45674.51408055556</v>
+        <v>45686.67839166667</v>
       </c>
       <c r="H62" s="1" t="n">
-        <v>45674.621325</v>
+        <v>45686.71403333333</v>
       </c>
       <c r="I62" s="1" t="n">
-        <v>45668.57291666666</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="63">
@@ -2736,19 +2736,19 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>D12X02570CU</t>
+          <t>D12X02230CU</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>437500</v>
+        <v>1236000</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2756,13 +2756,13 @@
         </is>
       </c>
       <c r="G63" s="1" t="n">
-        <v>45674.57646388889</v>
+        <v>45686.71504444444</v>
       </c>
       <c r="H63" s="1" t="n">
-        <v>45674.62897777778</v>
+        <v>45686.78733888889</v>
       </c>
       <c r="I63" s="1" t="n">
-        <v>45668.57291666666</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="64">
@@ -2773,19 +2773,19 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>MDW003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>D07X03090CU</t>
+          <t>D07X02570CU</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>598500</v>
+        <v>437500</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -2793,13 +2793,13 @@
         </is>
       </c>
       <c r="G64" s="1" t="n">
-        <v>45674.11040944445</v>
+        <v>45687.16455183333</v>
       </c>
       <c r="H64" s="1" t="n">
-        <v>45674.16228722222</v>
+        <v>45687.18645461111</v>
       </c>
       <c r="I64" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="65">
@@ -2810,19 +2810,19 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>MDW003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>D12X03090CU</t>
+          <t>D12X02570CU</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>598500</v>
+        <v>437500</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -2830,13 +2830,13 @@
         </is>
       </c>
       <c r="G65" s="1" t="n">
-        <v>45674.12676222222</v>
+        <v>45687.13394072223</v>
       </c>
       <c r="H65" s="1" t="n">
-        <v>45674.16228722222</v>
+        <v>45687.19219419445</v>
       </c>
       <c r="I65" s="1" t="n">
-        <v>45668.91319444445</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="66">
@@ -2851,15 +2851,15 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>D07X03560CU</t>
+          <t>D07X03090CU</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>9000</v>
+        <v>598500</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -2867,13 +2867,13 @@
         </is>
       </c>
       <c r="G66" s="1" t="n">
-        <v>45674.16242722223</v>
+        <v>45686.88731719444</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>45674.16330222222</v>
+        <v>45686.93919497222</v>
       </c>
       <c r="I66" s="1" t="n">
-        <v>45669.76597222222</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="67">
@@ -2888,15 +2888,15 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>D12X03560CU</t>
+          <t>D12X03090CU</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>9000</v>
+        <v>598500</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -2904,13 +2904,13 @@
         </is>
       </c>
       <c r="G67" s="1" t="n">
-        <v>45674.16242722223</v>
+        <v>45686.90366997222</v>
       </c>
       <c r="H67" s="1" t="n">
-        <v>45674.16330222222</v>
+        <v>45686.93919497222</v>
       </c>
       <c r="I67" s="1" t="n">
-        <v>45669.76597222222</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="68">
@@ -2925,15 +2925,15 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>D07X02840CU</t>
+          <t>D07X03560CU</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>180000</v>
+        <v>9000</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -2941,13 +2941,13 @@
         </is>
       </c>
       <c r="G68" s="1" t="n">
-        <v>45674.16355111111</v>
+        <v>45686.93933497222</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>45674.16871555556</v>
+        <v>45686.94020997222</v>
       </c>
       <c r="I68" s="1" t="n">
-        <v>45669.84375</v>
+        <v>45638.76597222222</v>
       </c>
     </row>
     <row r="69">
@@ -2962,15 +2962,15 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>D10X02840CU</t>
+          <t>D12X03560CU</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>540000</v>
+        <v>9000</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2978,13 +2978,13 @@
         </is>
       </c>
       <c r="G69" s="1" t="n">
-        <v>45674.16896444444</v>
+        <v>45686.93933497222</v>
       </c>
       <c r="H69" s="1" t="n">
-        <v>45674.19984222222</v>
+        <v>45686.94020997222</v>
       </c>
       <c r="I69" s="1" t="n">
-        <v>45669.84375</v>
+        <v>45638.76597222222</v>
       </c>
     </row>
     <row r="70">
@@ -2999,15 +2999,15 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>D12X02910CU</t>
+          <t>D07X02840CU</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>22500</v>
+        <v>180000</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -3015,13 +3015,13 @@
         </is>
       </c>
       <c r="G70" s="1" t="n">
-        <v>45674.20015805556</v>
+        <v>45686.78758777778</v>
       </c>
       <c r="H70" s="1" t="n">
-        <v>45674.20442180555</v>
+        <v>45686.79275222222</v>
       </c>
       <c r="I70" s="1" t="n">
-        <v>45669.95069444444</v>
+        <v>45638.84375</v>
       </c>
     </row>
     <row r="71">
@@ -3036,15 +3036,15 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>D08X02910CU</t>
+          <t>D10X02840CU</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>7500</v>
+        <v>540000</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -3052,13 +3052,13 @@
         </is>
       </c>
       <c r="G71" s="1" t="n">
-        <v>45674.20015805556</v>
+        <v>45686.79300111111</v>
       </c>
       <c r="H71" s="1" t="n">
-        <v>45674.20118930555</v>
+        <v>45686.82387888889</v>
       </c>
       <c r="I71" s="1" t="n">
-        <v>45669.95069444444</v>
+        <v>45638.84375</v>
       </c>
     </row>
     <row r="72">
@@ -3073,15 +3073,15 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>D14X02930CU</t>
+          <t>D12X02910CU</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>868400</v>
+        <v>22500</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -3089,13 +3089,13 @@
         </is>
       </c>
       <c r="G72" s="1" t="n">
-        <v>45674.20456180556</v>
+        <v>45686.82419472222</v>
       </c>
       <c r="H72" s="1" t="n">
-        <v>45674.25338991667</v>
+        <v>45686.82845847222</v>
       </c>
       <c r="I72" s="1" t="n">
-        <v>45670</v>
+        <v>45639.95069444444</v>
       </c>
     </row>
     <row r="73">
@@ -3110,29 +3110,103 @@
         </is>
       </c>
       <c r="C73" t="n">
+        <v>12</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>D08X02910CU</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>7500</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G73" s="1" t="n">
+        <v>45686.82419472222</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <v>45686.82522597222</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <v>45639.95069444444</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>MDW003</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>13</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>D14X02930CU</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>868400</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G74" s="1" t="n">
+        <v>45686.82859847222</v>
+      </c>
+      <c r="H74" s="1" t="n">
+        <v>45686.87742658333</v>
+      </c>
+      <c r="I74" s="1" t="n">
+        <v>45640</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>MDW003</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
         <v>14</v>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>D14X02930CU</t>
         </is>
       </c>
-      <c r="E73" t="n">
+      <c r="E75" t="n">
         <v>167400</v>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="G73" s="1" t="n">
-        <v>45674.25349880556</v>
-      </c>
-      <c r="H73" s="1" t="n">
-        <v>45674.26282941666</v>
-      </c>
-      <c r="I73" s="1" t="n">
-        <v>45670.10763888889</v>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G75" s="1" t="n">
+        <v>45686.87753547222</v>
+      </c>
+      <c r="H75" s="1" t="n">
+        <v>45686.88686608333</v>
+      </c>
+      <c r="I75" s="1" t="n">
+        <v>45640.10763888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saving commit (will document changes later)
</commit_message>
<xml_diff>
--- a/server/OUTPUT_MetalPlan.xlsx
+++ b/server/OUTPUT_MetalPlan.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BUN008</t>
+          <t>BUN025</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="G2" s="1" t="n">
-        <v>45689.10876496809</v>
+        <v>45722.09644444445</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>45691.64243497642</v>
+        <v>45723.76866666666</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>45635</v>
@@ -516,7 +516,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BUN054</t>
+          <t>BUN023</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>420000</v>
+        <v>490000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="G3" s="1" t="n">
-        <v>45688.16749069445</v>
+        <v>45720.69777777778</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>45690.62526847222</v>
+        <v>45723.60666666667</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>45635.09236111111</v>
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BUN024</t>
+          <t>BUN007</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>630000</v>
+        <v>560000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -573,10 +573,10 @@
         </is>
       </c>
       <c r="G4" s="1" t="n">
-        <v>45686.84194322222</v>
+        <v>45720.39555555556</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>45690.23749933334</v>
+        <v>45723.69333333334</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>45635.09236111111</v>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>420000</v>
+        <v>700000</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="G5" s="1" t="n">
-        <v>45688.00480643979</v>
+        <v>45719.39555555556</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>45690.46258421757</v>
+        <v>45723.53333333333</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>45635.09236111111</v>
@@ -627,7 +627,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BUN023</t>
+          <t>BUN004</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>560000</v>
+        <v>280000</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="G6" s="1" t="n">
-        <v>45686.87598655555</v>
+        <v>45721.99738620556</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>45690.17376433333</v>
+        <v>45723.61516398333</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>45635.09236111111</v>
@@ -664,7 +664,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BUN001</t>
+          <t>BUN013</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>420000</v>
+        <v>560000</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="G7" s="1" t="n">
-        <v>45687.80589760306</v>
+        <v>45720.72599372778</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>45690.14931651694</v>
+        <v>45723.87032796667</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>45635.34652777778</v>
@@ -701,7 +701,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BUN015</t>
+          <t>BUN005</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>420000</v>
+        <v>560000</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -721,10 +721,10 @@
         </is>
       </c>
       <c r="G8" s="1" t="n">
-        <v>45688.58053703333</v>
+        <v>45721.03845506111</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>45690.92395594722</v>
+        <v>45724.1827893</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>45635.34652777778</v>
@@ -738,7 +738,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BUN012</t>
+          <t>BUN010</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>560000</v>
+        <v>280000</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -758,10 +758,10 @@
         </is>
       </c>
       <c r="G9" s="1" t="n">
-        <v>45687.09571595</v>
+        <v>45722.20110732528</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>45690.24005018889</v>
+        <v>45723.74361091416</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>45635.34652777778</v>
@@ -775,7 +775,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BUN014</t>
+          <t>BUN006</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>171500</v>
+        <v>731500</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="G10" s="1" t="n">
-        <v>45686.9748115332</v>
+        <v>45720.34668192208</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>45687.94258421757</v>
+        <v>45724.51811590646</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>45635.34652777778</v>
@@ -812,7 +812,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BUN013</t>
+          <t>BUN003</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -824,7 +824,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>560000</v>
+        <v>700000</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -832,10 +832,10 @@
         </is>
       </c>
       <c r="G11" s="1" t="n">
-        <v>45686.99936222778</v>
+        <v>45720.39266039444</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>45690.14369646666</v>
+        <v>45724.33790995833</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>45635.34652777778</v>
@@ -849,7 +849,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BUN003</t>
+          <t>BUN024</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>280000</v>
+        <v>560000</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -869,10 +869,10 @@
         </is>
       </c>
       <c r="G12" s="1" t="n">
-        <v>45688.89269095</v>
+        <v>45720.72815</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>45690.43519453889</v>
+        <v>45723.98676666667</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>45635.34652777778</v>
@@ -886,7 +886,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BUN007</t>
+          <t>BUN012</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>560000</v>
+        <v>420000</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -906,10 +906,10 @@
         </is>
       </c>
       <c r="G13" s="1" t="n">
-        <v>45686.99936222778</v>
+        <v>45721.47266039444</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>45690.14369646666</v>
+        <v>45723.81607930833</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>45635.34652777778</v>
@@ -923,7 +923,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BUN006</t>
+          <t>BUN004</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>560000</v>
+        <v>280000</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -943,10 +943,10 @@
         </is>
       </c>
       <c r="G14" s="1" t="n">
-        <v>45687.71223306111</v>
+        <v>45720.39266039444</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>45690.8565673</v>
+        <v>45721.93516398333</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>45635.34652777778</v>
@@ -960,19 +960,19 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BUN004</t>
+          <t>BUN001</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>B0007X02570S023CU</t>
+          <t>B0007X02500S023SN</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>560000</v>
+        <v>375000</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -980,13 +980,13 @@
         </is>
       </c>
       <c r="G15" s="1" t="n">
-        <v>45686.99936222778</v>
+        <v>45722.66125247379</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>45690.14369646666</v>
+        <v>45724.85569691823</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45635.34652777778</v>
+        <v>45635.56458333333</v>
       </c>
     </row>
     <row r="16">
@@ -997,7 +997,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BUN015</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>250000</v>
+        <v>6000</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1017,10 +1017,10 @@
         </is>
       </c>
       <c r="G16" s="1" t="n">
-        <v>45687.07676552778</v>
+        <v>45719.66933333333</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>45688.52120997222</v>
+        <v>45719.70266666666</v>
       </c>
       <c r="I16" s="1" t="n">
         <v>45635.56458333333</v>
@@ -1034,19 +1034,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BUN006</t>
+          <t>BUN012</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>B0007X02500S023SN</t>
+          <t>B0019X01560S023CU</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>131000</v>
+        <v>180000</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1054,13 +1054,13 @@
         </is>
       </c>
       <c r="G17" s="1" t="n">
-        <v>45686.69551388889</v>
+        <v>45720.35777777778</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>45687.652906</v>
+        <v>45721.41333333333</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45635.56458333333</v>
+        <v>45636.45486111111</v>
       </c>
     </row>
     <row r="18">
@@ -1071,19 +1071,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BUN005</t>
+          <t>BUN009</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>B0019X01560S023CU</t>
+          <t>B0019X01835S025CU</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>125000</v>
+        <v>570000</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1091,13 +1091,13 @@
         </is>
       </c>
       <c r="G18" s="1" t="n">
-        <v>45689.22792711111</v>
+        <v>45720.84230050361</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>45689.92237155556</v>
+        <v>45723.91300745917</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45636.45486111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="19">
@@ -1108,19 +1108,19 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BUN012</t>
+          <t>BUN010</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>B0019X01560S023CU</t>
+          <t>B0019X01835S025CU</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>55000</v>
+        <v>190000</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1128,13 +1128,13 @@
         </is>
       </c>
       <c r="G19" s="1" t="n">
-        <v>45686.73083333333</v>
+        <v>45721.14380050361</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>45687.03638888889</v>
+        <v>45722.14178026417</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45636.45486111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="20">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BUN009</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>570000</v>
+        <v>475000</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1165,10 +1165,10 @@
         </is>
       </c>
       <c r="G20" s="1" t="n">
-        <v>45687.44077325361</v>
+        <v>45721.37067967028</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>45690.51148020917</v>
+        <v>45723.92320482709</v>
       </c>
       <c r="I20" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BUN010</t>
+          <t>BUN015</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1194,7 +1194,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>665000</v>
+        <v>380000</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1202,10 +1202,10 @@
         </is>
       </c>
       <c r="G21" s="1" t="n">
-        <v>45687.00349772583</v>
+        <v>45720.98044444445</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>45690.59238648014</v>
+        <v>45723.77766666667</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BUN001</t>
+          <t>BUN054</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>190000</v>
+        <v>285000</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         </is>
       </c>
       <c r="G22" s="1" t="n">
-        <v>45686.74859078139</v>
+        <v>45721.18833333333</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>45687.74657054195</v>
+        <v>45723.69</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BUN002</t>
+          <t>BUN011</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1268,7 +1268,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>380000</v>
+        <v>570000</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1276,10 +1276,10 @@
         </is>
       </c>
       <c r="G23" s="1" t="n">
-        <v>45688.4095328925</v>
+        <v>45720.76246717028</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>45690.44387625055</v>
+        <v>45723.83317412583</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BUN011</t>
+          <t>BUN001</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1305,7 +1305,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>665000</v>
+        <v>251600</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1313,10 +1313,10 @@
         </is>
       </c>
       <c r="G24" s="1" t="n">
-        <v>45687.30332828139</v>
+        <v>45721.25822222129</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>45690.8922170357</v>
+        <v>45722.60569691823</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BUN025</t>
+          <t>BUN002</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>285000</v>
+        <v>475000</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1350,10 +1350,10 @@
         </is>
       </c>
       <c r="G25" s="1" t="n">
-        <v>45688.12809330555</v>
+        <v>45721.34364217028</v>
       </c>
       <c r="H25" s="1" t="n">
-        <v>45690.62975997222</v>
+        <v>45723.89616732708</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BUN037</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>285000</v>
+        <v>190000</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1387,10 +1387,10 @@
         </is>
       </c>
       <c r="G26" s="1" t="n">
-        <v>45687.75282275</v>
+        <v>45721.23911111111</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>45690.25448941666</v>
+        <v>45723.43466666667</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1424,10 +1424,10 @@
         </is>
       </c>
       <c r="G27" s="1" t="n">
-        <v>45688.23861</v>
+        <v>45722.5065</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>45690.43416555555</v>
+        <v>45724.15316666666</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>45636.46736111111</v>
@@ -1441,19 +1441,19 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BUN008</t>
+          <t>BUN010</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>B0019X01835S025CU</t>
+          <t>B0019X02230S027CU</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>346600</v>
+        <v>585000</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1461,13 +1461,13 @@
         </is>
       </c>
       <c r="G28" s="1" t="n">
-        <v>45687.18586941573</v>
+        <v>45720.67027777778</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>45689.05152591143</v>
+        <v>45721.10541666667</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45636.46736111111</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="29">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BUN011</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>715000</v>
+        <v>130000</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1498,10 +1498,10 @@
         </is>
       </c>
       <c r="G29" s="1" t="n">
-        <v>45686.73230555555</v>
+        <v>45721.3165</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>45687.26494444445</v>
+        <v>45722.44316666666</v>
       </c>
       <c r="I29" s="1" t="n">
         <v>45636.54861111111</v>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BUN010</t>
+          <t>BUN011</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1527,7 +1527,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>325000</v>
+        <v>521000</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1535,10 +1535,10 @@
         </is>
       </c>
       <c r="G30" s="1" t="n">
-        <v>45686.724975</v>
+        <v>45720.33694444445</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>45686.96511388889</v>
+        <v>45720.72408333333</v>
       </c>
       <c r="I30" s="1" t="n">
         <v>45636.54861111111</v>
@@ -1552,19 +1552,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BUN003</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>B0019X02230S027CU</t>
+          <t>B0019X02570S030CU</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>196000</v>
+        <v>50000</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1572,13 +1572,13 @@
         </is>
       </c>
       <c r="G31" s="1" t="n">
-        <v>45686.76469722222</v>
+        <v>45721.05451805556</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>45688.48536388889</v>
+        <v>45721.33229583333</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>45636.54861111111</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="32">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BUN005</t>
+          <t>BUN002</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>237500</v>
+        <v>100000</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1609,10 +1609,10 @@
         </is>
       </c>
       <c r="G32" s="1" t="n">
-        <v>45687.76959377778</v>
+        <v>45720.72748055556</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>45689.17237155556</v>
+        <v>45721.30525833333</v>
       </c>
       <c r="I32" s="1" t="n">
         <v>45636.57291666666</v>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BUN002</t>
+          <t>BUN001</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1638,7 +1638,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1646,10 +1646,10 @@
         </is>
       </c>
       <c r="G33" s="1" t="n">
-        <v>45687.19337127778</v>
+        <v>45720.35555555556</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>45688.37114905556</v>
+        <v>45721.23333333333</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>45636.57291666666</v>
@@ -1663,19 +1663,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BUN037</t>
+          <t>BUN054</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>B0019X03090S035CU</t>
+          <t>B0019X02570S030CU</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>87000</v>
+        <v>50000</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1683,13 +1683,13 @@
         </is>
       </c>
       <c r="G34" s="1" t="n">
-        <v>45686.92582275</v>
+        <v>45720.70833333334</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>45687.68948941667</v>
+        <v>45721.125</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>45637.91319444445</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="35">
@@ -1700,19 +1700,19 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BUN009</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>B0019X03090S035CU</t>
+          <t>B0019X02570S030CU</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>116000</v>
+        <v>87500</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1720,13 +1720,13 @@
         </is>
       </c>
       <c r="G35" s="1" t="n">
-        <v>45686.91567275</v>
+        <v>45720.519</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>45687.40238941667</v>
+        <v>45721.27316666667</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>45637.91319444445</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="36">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BUN054</t>
+          <t>BUN008</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1749,7 +1749,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>58000</v>
+        <v>163500</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1757,10 +1757,10 @@
         </is>
       </c>
       <c r="G36" s="1" t="n">
-        <v>45687.60260180556</v>
+        <v>45720.34251666666</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>45688.10526847222</v>
+        <v>45721.03229583333</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>45637.91319444445</v>
@@ -1786,7 +1786,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>192500</v>
+        <v>232000</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1794,10 +1794,10 @@
         </is>
       </c>
       <c r="G37" s="1" t="n">
-        <v>45686.91798219444</v>
+        <v>45720.67955555556</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>45688.06475997222</v>
+        <v>45722.05866666666</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>45637.91319444445</v>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BUN003</t>
+          <t>BUN002</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>29000</v>
+        <v>87000</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1831,10 +1831,10 @@
         </is>
       </c>
       <c r="G38" s="1" t="n">
-        <v>45688.51114166667</v>
+        <v>45720.34251666666</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>45688.83336388889</v>
+        <v>45720.70525833334</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>45637.91319444445</v>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>BUN002</t>
+          <t>BUN037</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>58000</v>
+        <v>87000</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1868,10 +1868,10 @@
         </is>
       </c>
       <c r="G39" s="1" t="n">
-        <v>45686.91894330556</v>
+        <v>45719.722</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>45687.15770997222</v>
+        <v>45720.48566666667</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>45637.91319444445</v>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BUN008</t>
+          <t>BUN015</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>58000</v>
+        <v>29000</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1905,10 +1905,10 @@
         </is>
       </c>
       <c r="G40" s="1" t="n">
-        <v>45686.92221386111</v>
+        <v>45720.686</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>45687.16098052778</v>
+        <v>45720.92766666667</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>45637.91319444445</v>
@@ -1922,7 +1922,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BUN015</t>
+          <t>BUN009</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1942,10 +1942,10 @@
         </is>
       </c>
       <c r="G41" s="1" t="n">
-        <v>45686.94620997222</v>
+        <v>45720.72891666667</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>45687.02120997222</v>
+        <v>45720.80391666666</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>45638.76597222222</v>
@@ -1971,7 +1971,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>132000</v>
+        <v>116000</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1979,10 +1979,10 @@
         </is>
       </c>
       <c r="G42" s="1" t="n">
-        <v>45686.80211577778</v>
+        <v>45720.00395022222</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>45687.74737155555</v>
+        <v>45720.386628</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>45638.84375</v>
@@ -2008,7 +2008,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>48000</v>
+        <v>64000</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="G43" s="1" t="n">
-        <v>45686.80883222222</v>
+        <v>45720.58933333333</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>45687.23016555556</v>
+        <v>45721.15466666667</v>
       </c>
       <c r="I43" s="1" t="n">
         <v>45638.84375</v>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BUN008</t>
+          <t>BUN009</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -2053,10 +2053,10 @@
         </is>
       </c>
       <c r="G44" s="1" t="n">
-        <v>45686.83262513889</v>
+        <v>45720.67083333333</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>45686.88470847222</v>
+        <v>45720.72291666667</v>
       </c>
       <c r="I44" s="1" t="n">
         <v>45639.95069444444</v>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BUN054</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>100100</v>
+        <v>55100</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2090,10 +2090,10 @@
         </is>
       </c>
       <c r="G45" s="1" t="n">
-        <v>45686.83751847222</v>
+        <v>45719.67466666667</v>
       </c>
       <c r="H45" s="1" t="n">
-        <v>45687.58326847222</v>
+        <v>45720.32786666667</v>
       </c>
       <c r="I45" s="1" t="n">
         <v>45640</v>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>BUN054</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>63000</v>
+        <v>90000</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2127,10 +2127,10 @@
         </is>
       </c>
       <c r="G46" s="1" t="n">
-        <v>45687.40616555556</v>
+        <v>45720.005</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>45688.15416555556</v>
+        <v>45720.675</v>
       </c>
       <c r="I46" s="1" t="n">
         <v>45640</v>
@@ -2156,7 +2156,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>54000</v>
+        <v>72000</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2164,10 +2164,10 @@
         </is>
       </c>
       <c r="G47" s="1" t="n">
-        <v>45687.22738355555</v>
+        <v>45720.391628</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>45687.62738355555</v>
+        <v>45720.926628</v>
       </c>
       <c r="I47" s="1" t="n">
         <v>45640</v>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BMC003</t>
+          <t>BUN005</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>14000</v>
+        <v>7000</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2201,10 +2201,10 @@
         </is>
       </c>
       <c r="G48" s="1" t="n">
-        <v>45687.23638777778</v>
+        <v>45720.93051688889</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>45687.39816555555</v>
+        <v>45720.979128</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>45640.10763888889</v>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BUN005</t>
+          <t>BMC003</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>13900</v>
+        <v>20900</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2238,10 +2238,10 @@
         </is>
       </c>
       <c r="G49" s="1" t="n">
-        <v>45687.12196688889</v>
+        <v>45720.33408888889</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>45687.22238355556</v>
+        <v>45720.57866666667</v>
       </c>
       <c r="I49" s="1" t="n">
         <v>45640.10763888889</v>
@@ -2275,10 +2275,10 @@
         </is>
       </c>
       <c r="G50" s="1" t="n">
-        <v>45686.67066666667</v>
+        <v>45714.60397777778</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>45686.69566666667</v>
+        <v>45714.62897777778</v>
       </c>
       <c r="I50" s="1" t="n">
         <v>45635</v>
@@ -2312,10 +2312,10 @@
         </is>
       </c>
       <c r="G51" s="1" t="n">
-        <v>45686.79529211111</v>
+        <v>45714.29223055555</v>
       </c>
       <c r="H51" s="1" t="n">
-        <v>45686.89947544444</v>
+        <v>45714.39641388889</v>
       </c>
       <c r="I51" s="1" t="n">
         <v>45635.09236111111</v>
@@ -2349,10 +2349,10 @@
         </is>
       </c>
       <c r="G52" s="1" t="n">
-        <v>45686.92156294444</v>
+        <v>45714.00295555555</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>45687.13288516667</v>
+        <v>45714.23570555555</v>
       </c>
       <c r="I52" s="1" t="n">
         <v>45635.34652777778</v>
@@ -2378,7 +2378,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>250000</v>
+        <v>381000</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2386,10 +2386,10 @@
         </is>
       </c>
       <c r="G53" s="1" t="n">
-        <v>45686.67027777778</v>
+        <v>45713.33694444445</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>45686.69284722222</v>
+        <v>45713.38569444444</v>
       </c>
       <c r="I53" s="1" t="n">
         <v>45635.56458333333</v>
@@ -2403,19 +2403,19 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW002</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>D07X02500SN</t>
+          <t>D07X01560CU</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>131000</v>
+        <v>180000</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2423,13 +2423,13 @@
         </is>
       </c>
       <c r="G54" s="1" t="n">
-        <v>45686.90211433333</v>
+        <v>45713.62485</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>45686.91860738889</v>
+        <v>45713.64741944445</v>
       </c>
       <c r="I54" s="1" t="n">
-        <v>45635.56458333333</v>
+        <v>45636.45486111111</v>
       </c>
     </row>
     <row r="55">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>D07X01560CU</t>
+          <t>D12X01560CU</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="G55" s="1" t="n">
-        <v>45686.69645833333</v>
+        <v>45713.59866944444</v>
       </c>
       <c r="H55" s="1" t="n">
-        <v>45686.71902777778</v>
+        <v>45713.62123888889</v>
       </c>
       <c r="I55" s="1" t="n">
         <v>45636.45486111111</v>
@@ -2477,19 +2477,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>MDW002</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>D12X01560CU</t>
+          <t>D07X01835CU</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>180000</v>
+        <v>3576600</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2497,13 +2497,13 @@
         </is>
       </c>
       <c r="G56" s="1" t="n">
-        <v>45686.67027777778</v>
+        <v>45714.41295972222</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>45686.69284722222</v>
+        <v>45714.59997777778</v>
       </c>
       <c r="I56" s="1" t="n">
-        <v>45636.45486111111</v>
+        <v>45636.46736111111</v>
       </c>
     </row>
     <row r="57">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>MDW003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>D07X01835CU</t>
+          <t>D12X01835CU</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>380000</v>
+        <v>190000</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2534,10 +2534,10 @@
         </is>
       </c>
       <c r="G57" s="1" t="n">
-        <v>45686.66814444445</v>
+        <v>45714.39841944444</v>
       </c>
       <c r="H57" s="1" t="n">
-        <v>45686.67738055556</v>
+        <v>45714.41095416667</v>
       </c>
       <c r="I57" s="1" t="n">
         <v>45636.46736111111</v>
@@ -2571,10 +2571,10 @@
         </is>
       </c>
       <c r="G58" s="1" t="n">
-        <v>45686.72103333334</v>
+        <v>45713.33533888889</v>
       </c>
       <c r="H58" s="1" t="n">
-        <v>45686.98075277778</v>
+        <v>45713.59505833333</v>
       </c>
       <c r="I58" s="1" t="n">
         <v>45636.46736111111</v>
@@ -2588,19 +2588,19 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>MDW002</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>D07X01835CU</t>
+          <t>D07X02230CU</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>1710000</v>
+        <v>1236000</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2608,13 +2608,13 @@
         </is>
       </c>
       <c r="G59" s="1" t="n">
-        <v>45686.98275833333</v>
+        <v>45713.48721552778</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>45687.06799444444</v>
+        <v>45713.52285719445</v>
       </c>
       <c r="I59" s="1" t="n">
-        <v>45636.46736111111</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="60">
@@ -2625,19 +2625,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>D07X01835CU</t>
+          <t>D12X02230CU</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1486600</v>
+        <v>1236000</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2645,13 +2645,13 @@
         </is>
       </c>
       <c r="G60" s="1" t="n">
-        <v>45686.7122125</v>
+        <v>45713.52386830556</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>45686.79233655555</v>
+        <v>45713.59616275</v>
       </c>
       <c r="I60" s="1" t="n">
-        <v>45636.46736111111</v>
+        <v>45636.54861111111</v>
       </c>
     </row>
     <row r="61">
@@ -2666,15 +2666,15 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>D12X01835CU</t>
+          <t>D07X02570CU</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>190000</v>
+        <v>437500</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2682,13 +2682,13 @@
         </is>
       </c>
       <c r="G61" s="1" t="n">
-        <v>45686.69767222222</v>
+        <v>45714.17437777778</v>
       </c>
       <c r="H61" s="1" t="n">
-        <v>45686.71020694444</v>
+        <v>45714.28162222222</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>45636.46736111111</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="62">
@@ -2699,19 +2699,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>MDW003</t>
+          <t>MDW004</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>D07X02230CU</t>
+          <t>D12X02570CU</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>1236000</v>
+        <v>437500</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2719,13 +2719,13 @@
         </is>
       </c>
       <c r="G62" s="1" t="n">
-        <v>45686.67839166667</v>
+        <v>45714.23676111111</v>
       </c>
       <c r="H62" s="1" t="n">
-        <v>45686.71403333333</v>
+        <v>45714.289275</v>
       </c>
       <c r="I62" s="1" t="n">
-        <v>45636.54861111111</v>
+        <v>45636.57291666666</v>
       </c>
     </row>
     <row r="63">
@@ -2740,15 +2740,15 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>D12X02230CU</t>
+          <t>D07X03090CU</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1236000</v>
+        <v>598500</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2756,13 +2756,13 @@
         </is>
       </c>
       <c r="G63" s="1" t="n">
-        <v>45686.71504444444</v>
+        <v>45713.33479944444</v>
       </c>
       <c r="H63" s="1" t="n">
-        <v>45686.78733888889</v>
+        <v>45713.38667722222</v>
       </c>
       <c r="I63" s="1" t="n">
-        <v>45636.54861111111</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="64">
@@ -2773,19 +2773,19 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>D07X02570CU</t>
+          <t>D12X03090CU</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>437500</v>
+        <v>598500</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -2793,13 +2793,13 @@
         </is>
       </c>
       <c r="G64" s="1" t="n">
-        <v>45687.16455183333</v>
+        <v>45713.35115222223</v>
       </c>
       <c r="H64" s="1" t="n">
-        <v>45687.18645461111</v>
+        <v>45713.38667722222</v>
       </c>
       <c r="I64" s="1" t="n">
-        <v>45636.57291666666</v>
+        <v>45637.91319444445</v>
       </c>
     </row>
     <row r="65">
@@ -2810,19 +2810,19 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>MDW004</t>
+          <t>MDW003</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>D12X02570CU</t>
+          <t>D07X03560CU</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>437500</v>
+        <v>9000</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -2830,13 +2830,13 @@
         </is>
       </c>
       <c r="G65" s="1" t="n">
-        <v>45687.13394072223</v>
+        <v>45713.33347333333</v>
       </c>
       <c r="H65" s="1" t="n">
-        <v>45687.19219419445</v>
+        <v>45713.33434833333</v>
       </c>
       <c r="I65" s="1" t="n">
-        <v>45636.57291666666</v>
+        <v>45638.76597222222</v>
       </c>
     </row>
     <row r="66">
@@ -2851,15 +2851,15 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>D07X03090CU</t>
+          <t>D12X03560CU</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>598500</v>
+        <v>9000</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -2867,13 +2867,13 @@
         </is>
       </c>
       <c r="G66" s="1" t="n">
-        <v>45686.88731719444</v>
+        <v>45713.33347333333</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>45686.93919497222</v>
+        <v>45713.33434833333</v>
       </c>
       <c r="I66" s="1" t="n">
-        <v>45637.91319444445</v>
+        <v>45638.76597222222</v>
       </c>
     </row>
     <row r="67">
@@ -2888,15 +2888,15 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>D12X03090CU</t>
+          <t>D07X02840CU</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>598500</v>
+        <v>180000</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -2904,13 +2904,13 @@
         </is>
       </c>
       <c r="G67" s="1" t="n">
-        <v>45686.90366997222</v>
+        <v>45713.44991330556</v>
       </c>
       <c r="H67" s="1" t="n">
-        <v>45686.93919497222</v>
+        <v>45713.45507775</v>
       </c>
       <c r="I67" s="1" t="n">
-        <v>45637.91319444445</v>
+        <v>45638.84375</v>
       </c>
     </row>
     <row r="68">
@@ -2925,15 +2925,15 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>D07X03560CU</t>
+          <t>D10X02840CU</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>9000</v>
+        <v>540000</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -2941,13 +2941,13 @@
         </is>
       </c>
       <c r="G68" s="1" t="n">
-        <v>45686.93933497222</v>
+        <v>45713.45532663889</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>45686.94020997222</v>
+        <v>45713.48620441667</v>
       </c>
       <c r="I68" s="1" t="n">
-        <v>45638.76597222222</v>
+        <v>45638.84375</v>
       </c>
     </row>
     <row r="69">
@@ -2962,15 +2962,15 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>D12X03560CU</t>
+          <t>D12X02910CU</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>9000</v>
+        <v>22500</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2978,13 +2978,13 @@
         </is>
       </c>
       <c r="G69" s="1" t="n">
-        <v>45686.93933497222</v>
+        <v>45713.44540066666</v>
       </c>
       <c r="H69" s="1" t="n">
-        <v>45686.94020997222</v>
+        <v>45713.44966441666</v>
       </c>
       <c r="I69" s="1" t="n">
-        <v>45638.76597222222</v>
+        <v>45639.95069444444</v>
       </c>
     </row>
     <row r="70">
@@ -2999,15 +2999,15 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>D07X02840CU</t>
+          <t>D08X02910CU</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>180000</v>
+        <v>7500</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -3015,13 +3015,13 @@
         </is>
       </c>
       <c r="G70" s="1" t="n">
-        <v>45686.78758777778</v>
+        <v>45713.44540066666</v>
       </c>
       <c r="H70" s="1" t="n">
-        <v>45686.79275222222</v>
+        <v>45713.44643191667</v>
       </c>
       <c r="I70" s="1" t="n">
-        <v>45638.84375</v>
+        <v>45639.95069444444</v>
       </c>
     </row>
     <row r="71">
@@ -3036,15 +3036,15 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>D10X02840CU</t>
+          <t>D14X02930CU</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>540000</v>
+        <v>868400</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -3052,13 +3052,13 @@
         </is>
       </c>
       <c r="G71" s="1" t="n">
-        <v>45686.79300111111</v>
+        <v>45713.38681722222</v>
       </c>
       <c r="H71" s="1" t="n">
-        <v>45686.82387888889</v>
+        <v>45713.43564533333</v>
       </c>
       <c r="I71" s="1" t="n">
-        <v>45638.84375</v>
+        <v>45640</v>
       </c>
     </row>
     <row r="72">
@@ -3073,15 +3073,15 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>D12X02910CU</t>
+          <t>D14X02930CU</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>22500</v>
+        <v>167400</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -3089,123 +3089,12 @@
         </is>
       </c>
       <c r="G72" s="1" t="n">
-        <v>45686.82419472222</v>
+        <v>45713.43575422222</v>
       </c>
       <c r="H72" s="1" t="n">
-        <v>45686.82845847222</v>
+        <v>45713.44508483334</v>
       </c>
       <c r="I72" s="1" t="n">
-        <v>45639.95069444444</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>MDW003</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
-        <v>12</v>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>D08X02910CU</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>7500</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="G73" s="1" t="n">
-        <v>45686.82419472222</v>
-      </c>
-      <c r="H73" s="1" t="n">
-        <v>45686.82522597222</v>
-      </c>
-      <c r="I73" s="1" t="n">
-        <v>45639.95069444444</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>MDW003</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>13</v>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>D14X02930CU</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>868400</v>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="G74" s="1" t="n">
-        <v>45686.82859847222</v>
-      </c>
-      <c r="H74" s="1" t="n">
-        <v>45686.87742658333</v>
-      </c>
-      <c r="I74" s="1" t="n">
-        <v>45640</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>MDW003</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>14</v>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>D14X02930CU</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>167400</v>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="G75" s="1" t="n">
-        <v>45686.87753547222</v>
-      </c>
-      <c r="H75" s="1" t="n">
-        <v>45686.88686608333</v>
-      </c>
-      <c r="I75" s="1" t="n">
         <v>45640.10763888889</v>
       </c>
     </row>

</xml_diff>